<commit_message>
Changes resulting from sprint 11 alignment
</commit_message>
<xml_diff>
--- a/source_data/Roche Phase 3 NCT04320615.xlsx
+++ b/source_data/Roche Phase 3 NCT04320615.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/timepoints/source_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm_data/source_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{714B62EE-7AC9-6B40-900F-E76247405AF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EEAE84B-55E1-8B49-86EF-2768023BC062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45060" yWindow="7800" windowWidth="56520" windowHeight="19480" activeTab="2" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="45060" yWindow="7800" windowWidth="56520" windowHeight="19480" activeTab="8" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1720" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1726" uniqueCount="335">
   <si>
     <t>Epoch</t>
   </si>
@@ -1034,6 +1034,24 @@
   </si>
   <si>
     <t>The main design for the study</t>
+  </si>
+  <si>
+    <t>procedureName</t>
+  </si>
+  <si>
+    <t>procedureDescription</t>
+  </si>
+  <si>
+    <t>Test8</t>
+  </si>
+  <si>
+    <t>Test Eight</t>
+  </si>
+  <si>
+    <t>Test9</t>
+  </si>
+  <si>
+    <t>Test Nine</t>
   </si>
 </sst>
 </file>
@@ -1202,10 +1220,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2741,7 +2759,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57AA03AF-8646-874D-935F-A73550A0FA0C}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
       <selection activeCell="B3" sqref="B3:F3"/>
     </sheetView>
   </sheetViews>
@@ -2755,49 +2773,49 @@
       <c r="A1" s="26" t="s">
         <v>325</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="32" t="s">
         <v>326</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
         <v>327</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="32" t="s">
         <v>328</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
     </row>
     <row r="3" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="33" t="s">
         <v>236</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
     </row>
     <row r="4" spans="1:6" ht="160" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="33" t="s">
         <v>248</v>
       </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
@@ -2814,54 +2832,54 @@
       <c r="A6" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="32" t="s">
         <v>221</v>
       </c>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="32" t="s">
         <v>222</v>
       </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="B9" s="33" t="s">
+      <c r="B9" s="32" t="s">
         <v>228</v>
       </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="B10" s="33"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="8"/>
@@ -2932,16 +2950,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7654,69 +7672,89 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B29E6393-3A18-464C-A40D-B41879707264}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.33203125" customWidth="1"/>
-    <col min="2" max="2" width="17.5" customWidth="1"/>
-    <col min="3" max="3" width="27.33203125" customWidth="1"/>
-    <col min="4" max="4" width="24" style="29" customWidth="1"/>
-    <col min="5" max="5" width="29.6640625" customWidth="1"/>
-    <col min="6" max="6" width="14.83203125" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" customWidth="1"/>
+    <col min="4" max="4" width="17.5" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" customWidth="1"/>
+    <col min="6" max="6" width="24" style="29" customWidth="1"/>
+    <col min="7" max="7" width="29.6640625" customWidth="1"/>
+    <col min="8" max="8" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>182</v>
       </c>
       <c r="B1" s="27" t="s">
+        <v>329</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>330</v>
+      </c>
+      <c r="D1" s="27" t="s">
         <v>237</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="E1" s="27" t="s">
         <v>238</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="F1" s="28" t="s">
         <v>239</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="G1" s="27" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>241</v>
       </c>
       <c r="B2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C2" t="s">
+        <v>332</v>
+      </c>
+      <c r="D2" t="s">
         <v>242</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>244</v>
       </c>
       <c r="B3" t="s">
+        <v>333</v>
+      </c>
+      <c r="C3" t="s">
+        <v>334</v>
+      </c>
+      <c r="D3" t="s">
         <v>242</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>245</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="F3" s="29" t="s">
         <v>246</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="5"/>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D5" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>